<commit_message>
Revert "Se hicieron cambios en visualizaciones"
This reverts commit d8ed05444bed2a7c5c1d99064690d1f9ecdf5f34, reversing
changes made to 710d04f4632fc28b8dbc8f274efbb4b033e47a8c.
</commit_message>
<xml_diff>
--- a/data/clean/data_quality_report_CLEAN.xlsx
+++ b/data/clean/data_quality_report_CLEAN.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="25">
   <si>
     <t>Columna</t>
   </si>
@@ -38,9 +38,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>phone</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
@@ -74,10 +71,7 @@
     <t>N/A/N/A</t>
   </si>
   <si>
-    <t>0/258</t>
-  </si>
-  <si>
-    <t>1/258</t>
+    <t>0/1000</t>
   </si>
   <si>
     <t>purchase_date</t>
@@ -453,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -478,13 +472,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -492,13 +486,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -506,13 +500,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -523,10 +517,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -537,38 +531,38 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -576,97 +570,27 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -698,156 +622,156 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
         <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>